<commit_message>
started moving scraping to separate file. Will be adding more functionalities
</commit_message>
<xml_diff>
--- a/output/abdulka01.xlsx
+++ b/output/abdulka01.xlsx
@@ -25,7 +25,7 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Team</t>
+    <t>Tm</t>
   </si>
   <si>
     <t>Lg</t>
@@ -5290,9 +5290,6 @@
       <c r="N60">
         <v>0</v>
       </c>
-      <c r="O60">
-        <v>0.056</v>
-      </c>
       <c r="P60">
         <v>9.1</v>
       </c>
@@ -5382,9 +5379,6 @@
       <c r="N61">
         <v>0</v>
       </c>
-      <c r="O61">
-        <v>0</v>
-      </c>
       <c r="P61">
         <v>9.1</v>
       </c>
@@ -5456,9 +5450,6 @@
       <c r="N62">
         <v>0</v>
       </c>
-      <c r="O62">
-        <v>-0.056</v>
-      </c>
       <c r="P62">
         <v>0</v>
       </c>
@@ -5755,9 +5746,6 @@
       <c r="N66">
         <v>0</v>
       </c>
-      <c r="O66">
-        <v>0.056</v>
-      </c>
       <c r="P66">
         <v>10.2</v>
       </c>
@@ -5844,9 +5832,6 @@
       <c r="N67">
         <v>0</v>
       </c>
-      <c r="O67">
-        <v>0</v>
-      </c>
       <c r="P67">
         <v>9.9</v>
       </c>
@@ -5917,9 +5902,6 @@
       </c>
       <c r="N68">
         <v>0</v>
-      </c>
-      <c r="O68">
-        <v>-0.056</v>
       </c>
       <c r="P68">
         <v>-0.2999999999999989</v>
@@ -10401,9 +10383,6 @@
       <c r="N60">
         <v>0</v>
       </c>
-      <c r="O60">
-        <v>0.056</v>
-      </c>
       <c r="P60">
         <v>9.5</v>
       </c>
@@ -10490,9 +10469,6 @@
       <c r="N61">
         <v>0</v>
       </c>
-      <c r="O61">
-        <v>0</v>
-      </c>
       <c r="P61">
         <v>9.4</v>
       </c>
@@ -10561,9 +10537,6 @@
       <c r="N62">
         <v>0</v>
       </c>
-      <c r="O62">
-        <v>-0.056</v>
-      </c>
       <c r="P62">
         <v>-0.09999999999999964</v>
       </c>
@@ -10848,9 +10821,6 @@
       <c r="N66">
         <v>0</v>
       </c>
-      <c r="O66">
-        <v>0.056</v>
-      </c>
       <c r="P66">
         <v>9.9</v>
       </c>
@@ -10934,9 +10904,6 @@
       <c r="N67">
         <v>0</v>
       </c>
-      <c r="O67">
-        <v>0</v>
-      </c>
       <c r="P67">
         <v>9.6</v>
       </c>
@@ -11004,9 +10971,6 @@
       </c>
       <c r="N68">
         <v>0</v>
-      </c>
-      <c r="O68">
-        <v>-0.056</v>
       </c>
       <c r="P68">
         <v>-0.3000000000000007</v>
@@ -15012,9 +14976,6 @@
       <c r="N48">
         <v>0</v>
       </c>
-      <c r="O48">
-        <v>0.056</v>
-      </c>
       <c r="P48">
         <v>12.3</v>
       </c>
@@ -15107,9 +15068,6 @@
       <c r="N49">
         <v>0</v>
       </c>
-      <c r="O49">
-        <v>0</v>
-      </c>
       <c r="P49">
         <v>12.5</v>
       </c>
@@ -15184,9 +15142,6 @@
       <c r="N50">
         <v>0</v>
       </c>
-      <c r="O50">
-        <v>-0.056</v>
-      </c>
       <c r="P50">
         <v>0.1999999999999993</v>
       </c>
@@ -15486,9 +15441,6 @@
       <c r="N54">
         <v>0</v>
       </c>
-      <c r="O54">
-        <v>0.056</v>
-      </c>
       <c r="P54">
         <v>12.4</v>
       </c>
@@ -15578,9 +15530,6 @@
       <c r="N55">
         <v>0</v>
       </c>
-      <c r="O55">
-        <v>0</v>
-      </c>
       <c r="P55">
         <v>12.7</v>
       </c>
@@ -15654,9 +15603,6 @@
       </c>
       <c r="N56">
         <v>0</v>
-      </c>
-      <c r="O56">
-        <v>-0.056</v>
       </c>
       <c r="P56">
         <v>0.2999999999999989</v>
@@ -17141,13 +17087,13 @@
         <v>0.13</v>
       </c>
       <c r="AA25">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="AB25">
         <v>1.3</v>
       </c>
       <c r="AC25">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="AD25">
         <v>0.2</v>
@@ -17206,13 +17152,13 @@
         <v>-0.127</v>
       </c>
       <c r="AA26">
-        <v>-4</v>
+        <v>-4.1</v>
       </c>
       <c r="AB26">
         <v>-1.6</v>
       </c>
       <c r="AC26">
-        <v>-5.500000000000001</v>
+        <v>-5.600000000000001</v>
       </c>
       <c r="AD26">
         <v>-6.3</v>
@@ -17381,7 +17327,7 @@
         <v>2.8</v>
       </c>
       <c r="AC28">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="AD28">
         <v>0.9</v>
@@ -17446,7 +17392,7 @@
         <v>-0.2000000000000002</v>
       </c>
       <c r="AC29">
-        <v>0.5</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="AD29">
         <v>-6.8</v>
@@ -17858,13 +17804,13 @@
         <v>0.159</v>
       </c>
       <c r="AA34">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="AB34">
         <v>1</v>
       </c>
       <c r="AC34">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="AD34">
         <v>0.2</v>
@@ -17926,13 +17872,13 @@
         <v>-0.07100000000000001</v>
       </c>
       <c r="AA35">
-        <v>-1.7</v>
+        <v>-1.8</v>
       </c>
       <c r="AB35">
         <v>-0.3999999999999999</v>
       </c>
       <c r="AC35">
-        <v>-2.1</v>
+        <v>-2.2</v>
       </c>
       <c r="AD35">
         <v>-5.899999999999999</v>
@@ -18104,7 +18050,7 @@
         <v>3</v>
       </c>
       <c r="AB37">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="AC37">
         <v>4.4</v>
@@ -18172,7 +18118,7 @@
         <v>-0.7999999999999998</v>
       </c>
       <c r="AB38">
-        <v>0.1000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="AC38">
         <v>-0.5999999999999996</v>

</xml_diff>